<commit_message>
reduxified get_items and add_items
</commit_message>
<xml_diff>
--- a/app_data/test_data.xlsx
+++ b/app_data/test_data.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Projects\hemedisapp\app_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{777832EC-6490-4208-9D89-77E4F5A2C36E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{84DD765B-4E72-4C57-A4BB-F0FC5AC7E3D5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="test_data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,18 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
   <si>
-    <t>NAME</t>
-  </si>
-  <si>
-    <t>UNIT</t>
-  </si>
-  <si>
-    <t>BP</t>
-  </si>
-  <si>
-    <t>SP</t>
-  </si>
-  <si>
     <t>kg</t>
   </si>
   <si>
@@ -114,9 +102,6 @@
     <t>Metal Spade</t>
   </si>
   <si>
-    <t>ALIASES</t>
-  </si>
-  <si>
     <t>Cutting disc</t>
   </si>
   <si>
@@ -165,9 +150,6 @@
     <t>roll</t>
   </si>
   <si>
-    <t>QTY</t>
-  </si>
-  <si>
     <t>Hammer</t>
   </si>
   <si>
@@ -193,6 +175,24 @@
   </si>
   <si>
     <t>polyfilla</t>
+  </si>
+  <si>
+    <t>itemName</t>
+  </si>
+  <si>
+    <t>purchaseCost</t>
+  </si>
+  <si>
+    <t>sellingPrice</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>aliases</t>
   </si>
 </sst>
 </file>
@@ -556,7 +556,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,27 +566,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>52</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B2">
         <v>33</v>
@@ -600,7 +600,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>12.5</v>
@@ -614,7 +614,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>2800</v>
@@ -626,12 +626,12 @@
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B5">
         <v>110</v>
@@ -645,7 +645,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B6">
         <v>11</v>
@@ -654,18 +654,18 @@
         <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <v>300</v>
       </c>
       <c r="F6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B7">
         <v>1950</v>
@@ -674,7 +674,7 @@
         <v>3000</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E7">
         <v>5</v>
@@ -682,7 +682,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B8">
         <v>1150</v>
@@ -691,7 +691,7 @@
         <v>100</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E8">
         <v>5</v>
@@ -699,7 +699,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B9">
         <v>200</v>
@@ -713,7 +713,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B10">
         <v>130</v>
@@ -727,7 +727,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>80</v>
@@ -741,7 +741,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B12">
         <v>900</v>
@@ -755,7 +755,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <v>5</v>
@@ -769,7 +769,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B14">
         <v>35</v>
@@ -783,7 +783,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B15">
         <v>20</v>
@@ -797,7 +797,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B16">
         <v>90</v>
@@ -811,7 +811,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B17">
         <v>110</v>
@@ -823,12 +823,12 @@
         <v>6</v>
       </c>
       <c r="F17" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B18">
         <v>200</v>
@@ -842,7 +842,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B19">
         <v>16</v>
@@ -856,7 +856,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B20">
         <v>130</v>
@@ -870,7 +870,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B21">
         <v>150</v>
@@ -884,7 +884,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B22">
         <v>250</v>
@@ -896,12 +896,12 @@
         <v>8</v>
       </c>
       <c r="F22" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B23">
         <v>220</v>
@@ -915,7 +915,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B24">
         <v>150</v>
@@ -929,7 +929,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B25">
         <v>650</v>
@@ -943,7 +943,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B26">
         <v>1800</v>
@@ -957,7 +957,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B27">
         <v>200</v>
@@ -971,7 +971,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B28">
         <v>350</v>
@@ -985,7 +985,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B29">
         <v>130</v>
@@ -994,7 +994,7 @@
         <v>220</v>
       </c>
       <c r="D29" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E29">
         <v>73</v>
@@ -1002,7 +1002,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B30">
         <v>40</v>
@@ -1014,12 +1014,12 @@
         <v>27</v>
       </c>
       <c r="F30" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B31">
         <v>150</v>
@@ -1033,7 +1033,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B32">
         <v>140</v>
@@ -1047,7 +1047,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B33">
         <v>27</v>
@@ -1059,12 +1059,12 @@
         <v>19</v>
       </c>
       <c r="F33" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B34">
         <v>35</v>
@@ -1078,7 +1078,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B35">
         <v>16</v>
@@ -1090,12 +1090,12 @@
         <v>35</v>
       </c>
       <c r="F35" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B36">
         <v>23</v>
@@ -1109,7 +1109,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B37">
         <v>35</v>
@@ -1123,7 +1123,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B38">
         <v>30</v>
@@ -1137,7 +1137,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B39">
         <v>340</v>
@@ -1151,7 +1151,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B40">
         <v>60</v>
@@ -1165,7 +1165,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B41">
         <v>600</v>
@@ -1174,7 +1174,7 @@
         <v>900</v>
       </c>
       <c r="D41" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E41">
         <v>3</v>
@@ -1182,7 +1182,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B42">
         <v>370</v>
@@ -1191,7 +1191,7 @@
         <v>550</v>
       </c>
       <c r="D42" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E42">
         <v>1</v>

</xml_diff>